<commit_message>
Cambio de llamado de excel y pdf
</commit_message>
<xml_diff>
--- a/informes-excel/Ana-Martinez.xlsx
+++ b/informes-excel/Ana-Martinez.xlsx
@@ -44,7 +44,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>489</t>
+    <t>171</t>
   </si>
   <si>
     <t>Programacion 4.5</t>
@@ -56,7 +56,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>431</t>
+    <t>350</t>
   </si>
 </sst>
 </file>
@@ -91,12 +91,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="CDFFC4"/>
+        <fgColor rgb="FFF8C4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="CDFFC4"/>
+        <fgColor rgb="FFF8C4"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>